<commit_message>
replace todos with actual descriptions. Fill in missing content in index.md
</commit_message>
<xml_diff>
--- a/output/CodeSystem-SPLASCHCaloriePercentageCategoryCS.xlsx
+++ b/output/CodeSystem-SPLASCHCaloriePercentageCategoryCS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-08T12:48:12-05:00</t>
+    <t>2021-12-08T13:27:26-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>todo</t>
+    <t>Category codes for calorie percentage observations</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>